<commit_message>
add results with dlm
</commit_message>
<xml_diff>
--- a/results/f1_score_numbers.xlsx
+++ b/results/f1_score_numbers.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L62"/>
+  <dimension ref="A1:O62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -494,6 +494,21 @@
           <t>precision_microsoft</t>
         </is>
       </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>microsoft_dlm</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>recall_microsoft_dlm</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>precision_microsoft_dlm</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -544,6 +559,17 @@
       <c r="L2" t="n">
         <v>1</v>
       </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>J'aimerais transférer 3564,00$ de mon compte chèque à mon compte d'épargne. J'aimerais verser 199$ à début de chaque mois sur mon compte Bell.</t>
+        </is>
+      </c>
+      <c r="N2" t="n">
+        <v>1</v>
+      </c>
+      <c r="O2" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -594,6 +620,17 @@
       <c r="L3" t="n">
         <v>1</v>
       </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>Transfert 6000,07$ 80 et 9971$ de mon compte, celi le 11 novembre.</t>
+        </is>
+      </c>
+      <c r="N3" t="n">
+        <v>0.8461538461538461</v>
+      </c>
+      <c r="O3" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -644,6 +681,17 @@
       <c r="L4" t="n">
         <v>1</v>
       </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>Transfert de 51766,00$ 6652$ de mon compte celi le 29 décembre une fois cette année.</t>
+        </is>
+      </c>
+      <c r="N4" t="n">
+        <v>1</v>
+      </c>
+      <c r="O4" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -694,6 +742,17 @@
       <c r="L5" t="n">
         <v>0.875</v>
       </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>Transfert 2013$ à mon compte air au 1 janvier 2022.</t>
+        </is>
+      </c>
+      <c r="N5" t="n">
+        <v>1</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0.875</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -744,6 +803,17 @@
       <c r="L6" t="n">
         <v>1</v>
       </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>Je veux faire un dépôt de 5243,00$ aussi 37000,04$ 65 le 18 novembre 2021.</t>
+        </is>
+      </c>
+      <c r="N6" t="n">
+        <v>0.9523809523809523</v>
+      </c>
+      <c r="O6" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -794,6 +864,17 @@
       <c r="L7" t="n">
         <v>1</v>
       </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>Je dois faire un transfert international de 3666$ à mon oncle à Québec, le 31 octobre 2021.</t>
+        </is>
+      </c>
+      <c r="N7" t="n">
+        <v>1</v>
+      </c>
+      <c r="O7" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -844,6 +925,17 @@
       <c r="L8" t="n">
         <v>1</v>
       </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>J'aimerais, c'est du lait. Un paiement mensuel de 27,55$ sous qui sera versé tous les 15 du mois à partir d'octobre.</t>
+        </is>
+      </c>
+      <c r="N8" t="n">
+        <v>1</v>
+      </c>
+      <c r="O8" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -894,6 +986,17 @@
       <c r="L9" t="n">
         <v>1</v>
       </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>J'aimerais, c'est du lait. Un paiement mensuel de 65,33$ sous qui sera versé tous les 29 du mois à partir de mars 2022.</t>
+        </is>
+      </c>
+      <c r="N9" t="n">
+        <v>1</v>
+      </c>
+      <c r="O9" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -944,6 +1047,17 @@
       <c r="L10" t="n">
         <v>1</v>
       </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>Transfert, 5000, quatre-vingts dollars à mon compte réer le 16 avril 2022.</t>
+        </is>
+      </c>
+      <c r="N10" t="n">
+        <v>0.8888888888888888</v>
+      </c>
+      <c r="O10" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -994,6 +1108,17 @@
       <c r="L11" t="n">
         <v>1</v>
       </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>Moi j'aimerais transférer 2077$ au à Trois-Rivières s'il vous plaît de mon compte américain le 18 décembre.</t>
+        </is>
+      </c>
+      <c r="N11" t="n">
+        <v>1</v>
+      </c>
+      <c r="O11" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1044,6 +1169,17 @@
       <c r="L12" t="n">
         <v>1</v>
       </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>Transfert 33112,00$, 33214$.</t>
+        </is>
+      </c>
+      <c r="N12" t="n">
+        <v>1</v>
+      </c>
+      <c r="O12" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1094,6 +1230,17 @@
       <c r="L13" t="n">
         <v>1</v>
       </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>J'aimerais transférer 4654$ de mon compte chèque à mon compte d'épargne, j'aimerais aussi verser 398$ à la fin de chaque mois sur mon compte Bell.</t>
+        </is>
+      </c>
+      <c r="N13" t="n">
+        <v>1</v>
+      </c>
+      <c r="O13" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1144,6 +1291,17 @@
       <c r="L14" t="n">
         <v>0.9285714285714286</v>
       </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>Transfère 8000,08$ 70 à mon contraire et à un autre 9071,56$ sous de mon quantité celi le 11 novembre.</t>
+        </is>
+      </c>
+      <c r="N14" t="n">
+        <v>0.9285714285714286</v>
+      </c>
+      <c r="O14" t="n">
+        <v>0.9285714285714286</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1194,6 +1352,17 @@
       <c r="L15" t="n">
         <v>1</v>
       </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>Transfert de 31910,00$ 4452$ de mon compte celi le 23 décembre une fois cette année.</t>
+        </is>
+      </c>
+      <c r="N15" t="n">
+        <v>1</v>
+      </c>
+      <c r="O15" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1244,6 +1413,17 @@
       <c r="L16" t="n">
         <v>0.875</v>
       </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>Transfert 5012$ à mon compte réer le 1 février 2022.</t>
+        </is>
+      </c>
+      <c r="N16" t="n">
+        <v>1</v>
+      </c>
+      <c r="O16" t="n">
+        <v>0.875</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1294,6 +1474,17 @@
       <c r="L17" t="n">
         <v>1</v>
       </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>Je vais faire un dépôt de 90243,01$ autre 39000,03$ 61, le 23 novembre 2021.</t>
+        </is>
+      </c>
+      <c r="N17" t="n">
+        <v>0.9583333333333334</v>
+      </c>
+      <c r="O17" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1344,6 +1535,17 @@
       <c r="L18" t="n">
         <v>1</v>
       </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>Je dois effectuer un transfert international de 8606$ à mon oncle à Paris le 30 juin 2021.</t>
+        </is>
+      </c>
+      <c r="N18" t="n">
+        <v>1</v>
+      </c>
+      <c r="O18" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1394,6 +1596,17 @@
       <c r="L19" t="n">
         <v>1</v>
       </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>J'aimerais du lait. Un paiement mensuel de 39,68$ sous qui sera versé tous les 28 du mois à partir d'octobre.</t>
+        </is>
+      </c>
+      <c r="N19" t="n">
+        <v>1</v>
+      </c>
+      <c r="O19" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1444,6 +1657,17 @@
       <c r="L20" t="n">
         <v>1</v>
       </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>J'aimerais céduler un paiement mensuel de 69,59$ sous qui sera versé tous les 14 du mois à partir de mars 2022.</t>
+        </is>
+      </c>
+      <c r="N20" t="n">
+        <v>1</v>
+      </c>
+      <c r="O20" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1494,6 +1718,17 @@
       <c r="L21" t="n">
         <v>1</v>
       </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>Transférer 31000 et 4$ à mon compte réer au 16 avril 2022.</t>
+        </is>
+      </c>
+      <c r="N21" t="n">
+        <v>1</v>
+      </c>
+      <c r="O21" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1544,6 +1779,17 @@
       <c r="L22" t="n">
         <v>1</v>
       </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>Moi, j'aimerais transférer 2078$ s'il vous plaît de mon compte américain le 17 décembre.</t>
+        </is>
+      </c>
+      <c r="N22" t="n">
+        <v>1</v>
+      </c>
+      <c r="O22" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1594,6 +1840,17 @@
       <c r="L23" t="n">
         <v>1</v>
       </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>Transférer, 35130,00$ aussi 33920$.</t>
+        </is>
+      </c>
+      <c r="N23" t="n">
+        <v>1</v>
+      </c>
+      <c r="O23" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1644,6 +1901,17 @@
       <c r="L24" t="n">
         <v>1</v>
       </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>Transférer 67030,00$ transférer aussi 25715,30$ sous.</t>
+        </is>
+      </c>
+      <c r="N24" t="n">
+        <v>1</v>
+      </c>
+      <c r="O24" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1694,6 +1962,17 @@
       <c r="L25" t="n">
         <v>1</v>
       </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>J'aimerais transférer 2834,00$ de mon compte chèque à mon compte d'épargne et j'aimerais aussi verser 295$ à la fin de chaque mois sur mon compte belle.</t>
+        </is>
+      </c>
+      <c r="N25" t="n">
+        <v>1</v>
+      </c>
+      <c r="O25" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1744,6 +2023,17 @@
       <c r="L26" t="n">
         <v>1</v>
       </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>Transfert 1000,00$ 10 et un autre 2072,12$ sous de mon compte celi le 20 novembre.</t>
+        </is>
+      </c>
+      <c r="N26" t="n">
+        <v>0.9090909090909091</v>
+      </c>
+      <c r="O26" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1794,6 +2084,17 @@
       <c r="L27" t="n">
         <v>1</v>
       </c>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>Transfert 21110,03$ 1455,00$ de mon compte celi le 2 décembre de cette année.</t>
+        </is>
+      </c>
+      <c r="N27" t="n">
+        <v>1</v>
+      </c>
+      <c r="O27" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1844,6 +2145,17 @@
       <c r="L28" t="n">
         <v>1</v>
       </c>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>Transfert, 13013$ à mon compte réel le 10 février 2022.</t>
+        </is>
+      </c>
+      <c r="N28" t="n">
+        <v>1</v>
+      </c>
+      <c r="O28" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1894,6 +2206,17 @@
       <c r="L29" t="n">
         <v>1</v>
       </c>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t>Je vais faire un dépôt de 81000 et 83,01$ autre transfert de 31000,09$ 160 et 3 le 30 novembre 2021.</t>
+        </is>
+      </c>
+      <c r="N29" t="n">
+        <v>1</v>
+      </c>
+      <c r="O29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1944,6 +2267,17 @@
       <c r="L30" t="n">
         <v>1</v>
       </c>
+      <c r="M30" t="inlineStr">
+        <is>
+          <t>Je dois effectuer un transfert Inter international de 9107$ à mon oncle le 30 juillet 2021.</t>
+        </is>
+      </c>
+      <c r="N30" t="n">
+        <v>1</v>
+      </c>
+      <c r="O30" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1994,6 +2328,17 @@
       <c r="L31" t="n">
         <v>1</v>
       </c>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>J'aimerais céduler un paiement mensuel de 32,18$ sous le 7 de chaque mois à partir d'octobre.</t>
+        </is>
+      </c>
+      <c r="N31" t="n">
+        <v>1</v>
+      </c>
+      <c r="O31" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -2044,6 +2389,17 @@
       <c r="L32" t="n">
         <v>0.9</v>
       </c>
+      <c r="M32" t="inlineStr">
+        <is>
+          <t>Je m'assis du lait un paiement mensuel de 49,49$ sous tous les 11 du mois à partir d'avril 2022.</t>
+        </is>
+      </c>
+      <c r="N32" t="n">
+        <v>1</v>
+      </c>
+      <c r="O32" t="n">
+        <v>0.9</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -2094,6 +2450,17 @@
       <c r="L33" t="n">
         <v>1</v>
       </c>
+      <c r="M33" t="inlineStr">
+        <is>
+          <t>Transfert 21000 et 99$ à mon compte réer au 3 avril 2022.</t>
+        </is>
+      </c>
+      <c r="N33" t="n">
+        <v>1</v>
+      </c>
+      <c r="O33" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -2144,6 +2511,17 @@
       <c r="L34" t="n">
         <v>1</v>
       </c>
+      <c r="M34" t="inlineStr">
+        <is>
+          <t>Moi, j'aimerais transférer 20079$ en Floride. S'il vous plaît de mon compte américain, le 31 décembre.</t>
+        </is>
+      </c>
+      <c r="N34" t="n">
+        <v>1</v>
+      </c>
+      <c r="O34" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -2194,6 +2572,17 @@
       <c r="L35" t="n">
         <v>1</v>
       </c>
+      <c r="M35" t="inlineStr">
+        <is>
+          <t>Transférer 6103,00$ 34410$.</t>
+        </is>
+      </c>
+      <c r="N35" t="n">
+        <v>1</v>
+      </c>
+      <c r="O35" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -2244,6 +2633,17 @@
       <c r="L36" t="n">
         <v>1</v>
       </c>
+      <c r="M36" t="inlineStr">
+        <is>
+          <t>Je voudrais transférer 1345,00$ aussi 2564$ à mon compte réer aujourd?</t>
+        </is>
+      </c>
+      <c r="N36" t="n">
+        <v>1</v>
+      </c>
+      <c r="O36" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -2294,6 +2694,17 @@
       <c r="L37" t="n">
         <v>1</v>
       </c>
+      <c r="M37" t="inlineStr">
+        <is>
+          <t>Je voudrais transférer 2898,00$ 1135$ sur mon compte, cpg demain.</t>
+        </is>
+      </c>
+      <c r="N37" t="n">
+        <v>1</v>
+      </c>
+      <c r="O37" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -2344,6 +2755,17 @@
       <c r="L38" t="n">
         <v>1</v>
       </c>
+      <c r="M38" t="inlineStr">
+        <is>
+          <t>Je voudrais changer mon nip à 66 77 88.</t>
+        </is>
+      </c>
+      <c r="N38" t="n">
+        <v>1</v>
+      </c>
+      <c r="O38" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -2394,6 +2816,17 @@
       <c r="L39" t="n">
         <v>1</v>
       </c>
+      <c r="M39" t="inlineStr">
+        <is>
+          <t>Je voudrais faire 3 transferts sur mon compte d'épargne BNC. Le premier montant est de 1234$, le 2nd de 2345,00$, le dernier de 3456,00$.</t>
+        </is>
+      </c>
+      <c r="N39" t="n">
+        <v>1</v>
+      </c>
+      <c r="O39" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -2444,6 +2877,17 @@
       <c r="L40" t="n">
         <v>1</v>
       </c>
+      <c r="M40" t="inlineStr">
+        <is>
+          <t>Je voudrais transférer 6677,00$ 7788,00$ sur mon compte cpg demain.</t>
+        </is>
+      </c>
+      <c r="N40" t="n">
+        <v>1</v>
+      </c>
+      <c r="O40" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -2494,6 +2938,17 @@
       <c r="L41" t="n">
         <v>1</v>
       </c>
+      <c r="M41" t="inlineStr">
+        <is>
+          <t>Je voudrais transférer 1001,00$ 2002$ sur mon compte, CPG demain.</t>
+        </is>
+      </c>
+      <c r="N41" t="n">
+        <v>1</v>
+      </c>
+      <c r="O41" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -2544,6 +2999,17 @@
       <c r="L42" t="n">
         <v>1</v>
       </c>
+      <c r="M42" t="inlineStr">
+        <is>
+          <t>Je voudrais transférer 20001,00$ 3005$ sur mon compte, CPG demain.</t>
+        </is>
+      </c>
+      <c r="N42" t="n">
+        <v>1</v>
+      </c>
+      <c r="O42" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -2594,6 +3060,17 @@
       <c r="L43" t="n">
         <v>1</v>
       </c>
+      <c r="M43" t="inlineStr">
+        <is>
+          <t>Je voudrais transférer 8888,07$ 1567$ sur mon compte, cpg demain.</t>
+        </is>
+      </c>
+      <c r="N43" t="n">
+        <v>1</v>
+      </c>
+      <c r="O43" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -2644,6 +3121,17 @@
       <c r="L44" t="n">
         <v>1</v>
       </c>
+      <c r="M44" t="inlineStr">
+        <is>
+          <t>J'aimerais, c'est du lait. Un paiement mensuel de 35,25$ sous qui sera versé tous les 17 du mois à partir d'octobre.</t>
+        </is>
+      </c>
+      <c r="N44" t="n">
+        <v>1</v>
+      </c>
+      <c r="O44" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -2694,6 +3182,17 @@
       <c r="L45" t="n">
         <v>1</v>
       </c>
+      <c r="M45" t="inlineStr">
+        <is>
+          <t>J'aimerais du lait. Un paiement mensuel de 68,35$ sous qui traversaient tous les 8 du mois à partir d'octobre.</t>
+        </is>
+      </c>
+      <c r="N45" t="n">
+        <v>1</v>
+      </c>
+      <c r="O45" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -2744,6 +3243,17 @@
       <c r="L46" t="n">
         <v>1</v>
       </c>
+      <c r="M46" t="inlineStr">
+        <is>
+          <t>J'aimerais céduler un paiement mensuel de 58,09$ sous qui sera versé tous les premiers du mois à partir d'octobre.</t>
+        </is>
+      </c>
+      <c r="N46" t="n">
+        <v>1</v>
+      </c>
+      <c r="O46" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -2794,6 +3304,17 @@
       <c r="L47" t="n">
         <v>1</v>
       </c>
+      <c r="M47" t="inlineStr">
+        <is>
+          <t>Je voudrais faire 3 transferts sur mon compte d'épargne BNC. Le premier montant est de soi 65343$. Le 2nd de 2999,00$, le dernier de 20,00$.</t>
+        </is>
+      </c>
+      <c r="N47" t="n">
+        <v>1</v>
+      </c>
+      <c r="O47" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -2844,6 +3365,17 @@
       <c r="L48" t="n">
         <v>1</v>
       </c>
+      <c r="M48" t="inlineStr">
+        <is>
+          <t>Je voudrais faire 3 transferts sur mon compte d'épargne BNC. Le premier montant est de 1234$, le 2nd de 2345,00$, le dernier de 3456,00$.</t>
+        </is>
+      </c>
+      <c r="N48" t="n">
+        <v>1</v>
+      </c>
+      <c r="O48" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -2894,6 +3426,17 @@
       <c r="L49" t="n">
         <v>1</v>
       </c>
+      <c r="M49" t="inlineStr">
+        <is>
+          <t>Je voudrais faire 5 transferts sur mon compte d'épargne BNC, le premier d'un montant de 10$, le 2nd de 20$ le 3e de 30,00$ le 4e de 40,00$ le 5e de 50$.</t>
+        </is>
+      </c>
+      <c r="N49" t="n">
+        <v>1</v>
+      </c>
+      <c r="O49" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -2944,6 +3487,17 @@
       <c r="L50" t="n">
         <v>1</v>
       </c>
+      <c r="M50" t="inlineStr">
+        <is>
+          <t>Je voudrais faire 5 transferts sur mon compte d'épargne BNC, le premier de 60$, le 2nd de 70,00$, le 3e de quatre-vingts dollars, le 4e de 90,00$, le 5e de 100$.</t>
+        </is>
+      </c>
+      <c r="N50" t="n">
+        <v>1</v>
+      </c>
+      <c r="O50" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -2994,6 +3548,17 @@
       <c r="L51" t="n">
         <v>1</v>
       </c>
+      <c r="M51" t="inlineStr">
+        <is>
+          <t>Je voudrais faire 5 transferts sur mon compte d'épargne BNC, le premier de 100,00$, le 2e de 200$, le 3e de 300$, le 4e de 400,00$, le 5e de 500$.</t>
+        </is>
+      </c>
+      <c r="N51" t="n">
+        <v>1</v>
+      </c>
+      <c r="O51" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -3044,6 +3609,17 @@
       <c r="L52" t="n">
         <v>1</v>
       </c>
+      <c r="M52" t="inlineStr">
+        <is>
+          <t>Je voudrais faire 5 virements sur mon compte d'épargne BC le premier de 600$, le 2e de 700$, le 3e de 800,00$, le 4e de 900,00$, le 5e de 1000 Do.</t>
+        </is>
+      </c>
+      <c r="N52" t="n">
+        <v>1</v>
+      </c>
+      <c r="O52" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -3094,6 +3670,17 @@
       <c r="L53" t="n">
         <v>1</v>
       </c>
+      <c r="M53" t="inlineStr">
+        <is>
+          <t>Je voudrais faire 5 transferts sur mon compte d'épargne BNC, le premier de 1001,00$, le 2e de 1010$, le 3e de 1100,00$, le 4e de 1110,00$, le 5e de 1111$.</t>
+        </is>
+      </c>
+      <c r="N53" t="n">
+        <v>1</v>
+      </c>
+      <c r="O53" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -3144,6 +3731,17 @@
       <c r="L54" t="n">
         <v>1</v>
       </c>
+      <c r="M54" t="inlineStr">
+        <is>
+          <t>Je voudrais faire 5 transferts sur mon compte d'épargne BNC, le premier pour 2001,00$ le 2e pour 2020$, le 3e pour 2200$, 4e pour 2220,00$, le 5e pour 2222$.</t>
+        </is>
+      </c>
+      <c r="N54" t="n">
+        <v>1</v>
+      </c>
+      <c r="O54" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -3194,6 +3792,17 @@
       <c r="L55" t="n">
         <v>1</v>
       </c>
+      <c r="M55" t="inlineStr">
+        <is>
+          <t>Je voudrais faire 5 transferts sur mon compte réer, le premier pour 3001,00$, le 2e pour 3030$, le 3e pour 3300$, le 4e pour 3330$, le 5e pour 3333$.</t>
+        </is>
+      </c>
+      <c r="N55" t="n">
+        <v>1</v>
+      </c>
+      <c r="O55" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -3244,6 +3853,17 @@
       <c r="L56" t="n">
         <v>1</v>
       </c>
+      <c r="M56" t="inlineStr">
+        <is>
+          <t>Je voudrais payer 13511$ à ma marge de crédit.</t>
+        </is>
+      </c>
+      <c r="N56" t="n">
+        <v>1</v>
+      </c>
+      <c r="O56" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -3294,6 +3914,17 @@
       <c r="L57" t="n">
         <v>1</v>
       </c>
+      <c r="M57" t="inlineStr">
+        <is>
+          <t>Je voudrais payer 13533$ à ma marge de crédit.</t>
+        </is>
+      </c>
+      <c r="N57" t="n">
+        <v>1</v>
+      </c>
+      <c r="O57" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -3344,6 +3975,17 @@
       <c r="L58" t="n">
         <v>1</v>
       </c>
+      <c r="M58" t="inlineStr">
+        <is>
+          <t>Je voudrais payer 13555$ à ma marge de crédit.</t>
+        </is>
+      </c>
+      <c r="N58" t="n">
+        <v>1</v>
+      </c>
+      <c r="O58" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -3394,6 +4036,17 @@
       <c r="L59" t="n">
         <v>1</v>
       </c>
+      <c r="M59" t="inlineStr">
+        <is>
+          <t>Je voudrais payer 13566$ à ma marge de crédit.</t>
+        </is>
+      </c>
+      <c r="N59" t="n">
+        <v>1</v>
+      </c>
+      <c r="O59" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -3444,6 +4097,17 @@
       <c r="L60" t="n">
         <v>1</v>
       </c>
+      <c r="M60" t="inlineStr">
+        <is>
+          <t>Je voudrais payer 13577$ à ma marge de crédit.</t>
+        </is>
+      </c>
+      <c r="N60" t="n">
+        <v>1</v>
+      </c>
+      <c r="O60" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -3494,6 +4158,17 @@
       <c r="L61" t="n">
         <v>1</v>
       </c>
+      <c r="M61" t="inlineStr">
+        <is>
+          <t>Je voudrais payer 13588$ à ma marge de crédit.</t>
+        </is>
+      </c>
+      <c r="N61" t="n">
+        <v>1</v>
+      </c>
+      <c r="O61" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -3542,6 +4217,17 @@
         <v>1</v>
       </c>
       <c r="L62" t="n">
+        <v>1</v>
+      </c>
+      <c r="M62" t="inlineStr">
+        <is>
+          <t>Je voudrais payer 13599$ à ma marge de crédit.</t>
+        </is>
+      </c>
+      <c r="N62" t="n">
+        <v>1</v>
+      </c>
+      <c r="O62" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>